<commit_message>
Added more testcases and fixed failure testcases navigation to reset for next testcase.
</commit_message>
<xml_diff>
--- a/selenium-samples/TestData/TestPortalData.xlsx
+++ b/selenium-samples/TestData/TestPortalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a48587250d8e8ac/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{04858E79-B85A-4694-AC10-C7F0F7ECCE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E97A908D-7461-47C1-89AE-C94475E1DC97}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{04858E79-B85A-4694-AC10-C7F0F7ECCE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C522981A-7999-405C-892C-F4737E828648}"/>
   <bookViews>
-    <workbookView xWindow="1668" yWindow="948" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{3687BB54-7277-4634-9976-B728E366D08D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3687BB54-7277-4634-9976-B728E366D08D}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -68,16 +68,48 @@
   </si>
   <si>
     <t>5085 4600 3187 8112</t>
+  </si>
+  <si>
+    <t>demo12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   demo12  </t>
+  </si>
+  <si>
+    <t>DEMO12</t>
+  </si>
+  <si>
+    <t>#$%$#@</t>
+  </si>
+  <si>
+    <t>&lt;!--Demo12--!&gt;</t>
+  </si>
+  <si>
+    <t>Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;Demo12kflkvjflkvflkjoi4j5tkefelflaefkevmkldflkal;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">               </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,14 +132,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85CEF5B-89C5-474B-8494-DAF43E926C13}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,7 +519,81 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" xr:uid="{E515B4C1-7549-4CE4-95D3-40745014373B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -514,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4020FB22-8575-457B-8721-1B687CBAF149}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>